<commit_message>
maj de l'excel version utilisable
</commit_message>
<xml_diff>
--- a/data/climate_data/indicateurs_pedologiques/191021_Indicators_Dev_Meta_Network - Version_utilisable.xlsx
+++ b/data/climate_data/indicateurs_pedologiques/191021_Indicators_Dev_Meta_Network - Version_utilisable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN.RDS-PRET-0218\Desktop\Agrocampus Ouest\M2\Projet ingénieur\meteo_vs_rendement\data\climate_data\indicateurs_pedologiques\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81DF8CFA-1600-49AE-89BD-7499A6AF2F7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ED18ADE-4E7D-4B76-84EE-1546EDCBAD48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -382,7 +382,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="260">
   <si>
     <t>PROJET</t>
   </si>
@@ -885,12 +885,6 @@
     <t>F_W_WSC_MAX</t>
   </si>
   <si>
-    <t>F_W_WSN_MN(%)</t>
-  </si>
-  <si>
-    <t>F_W_WSC_MN(mm)</t>
-  </si>
-  <si>
     <t>F_S_SSR</t>
   </si>
   <si>
@@ -922,12 +916,6 @@
   </si>
   <si>
     <t>CW_W_WS</t>
-  </si>
-  <si>
-    <t>CW_W_WSN_MN(%)</t>
-  </si>
-  <si>
-    <t>CW_W_WSC_MN(mm)</t>
   </si>
   <si>
     <t>CW_S_SSR</t>
@@ -966,19 +954,10 @@
     <t>B_W_WS</t>
   </si>
   <si>
-    <t>B_W_WSN_MN(%)</t>
-  </si>
-  <si>
-    <t>B_W_WSC_MN(mm)</t>
-  </si>
-  <si>
     <t>B_S_SSR</t>
   </si>
   <si>
     <t>B_S_LSR</t>
-  </si>
-  <si>
-    <t>F_S_QPT</t>
   </si>
   <si>
     <t>P300_T_TMIN</t>
@@ -1035,12 +1014,6 @@
     <t>P600_W_WS</t>
   </si>
   <si>
-    <t>P600_W_WSN_MN(%)</t>
-  </si>
-  <si>
-    <t>P600_W_WSC_MN(mm)</t>
-  </si>
-  <si>
     <t>P600_S_SSR</t>
   </si>
   <si>
@@ -1071,9 +1044,6 @@
     <t>P1000_W_WS</t>
   </si>
   <si>
-    <t>P1000_W_WSN_MN(%)</t>
-  </si>
-  <si>
     <t>P1000_S_SSR</t>
   </si>
   <si>
@@ -1092,9 +1062,6 @@
     <t>N_N_NI</t>
   </si>
   <si>
-    <t>N_WN_WSC_I</t>
-  </si>
-  <si>
     <t>N_WN_BI_DRY</t>
   </si>
   <si>
@@ -1110,19 +1077,91 @@
     <t>N_N_N_Sol</t>
   </si>
   <si>
-    <t>N_WN_WSC_I(%)</t>
+    <t>DELTA DTF</t>
   </si>
   <si>
-    <t>P300_W_WSN_MN(%)</t>
+    <t>FLO_T_TMIN</t>
   </si>
   <si>
-    <t>P300_W_WSC_MN(mm)</t>
+    <t>FLO_T_TMAX</t>
   </si>
   <si>
-    <t>P1000_W_WSC_MN(mm)</t>
+    <t>FLO_T_TMN</t>
   </si>
   <si>
-    <t>DELTA DTF</t>
+    <t>FLO_T_FR</t>
+  </si>
+  <si>
+    <t>FLO_T_HT</t>
+  </si>
+  <si>
+    <t>FLO_T_LT</t>
+  </si>
+  <si>
+    <t>FLO_T_LGDD</t>
+  </si>
+  <si>
+    <t>FLO_W_WD</t>
+  </si>
+  <si>
+    <t>FLO_W_WS</t>
+  </si>
+  <si>
+    <t>FLO_S_SSR</t>
+  </si>
+  <si>
+    <t>FLO_S_LSR</t>
+  </si>
+  <si>
+    <t>FLO_S_QPT</t>
+  </si>
+  <si>
+    <t>F_W_WSN_MN</t>
+  </si>
+  <si>
+    <t>F_W_WSC_MN</t>
+  </si>
+  <si>
+    <t>CW_W_WSN_MN</t>
+  </si>
+  <si>
+    <t>CW_W_WSC_MN</t>
+  </si>
+  <si>
+    <t>B_W_WSN_MN</t>
+  </si>
+  <si>
+    <t>B_W_WSC_MN</t>
+  </si>
+  <si>
+    <t>FLO_W_WSN_MN</t>
+  </si>
+  <si>
+    <t>FLO_W_WSC_MN</t>
+  </si>
+  <si>
+    <t>P300_W_WSC_MN</t>
+  </si>
+  <si>
+    <t>P300_W_WSN_MN</t>
+  </si>
+  <si>
+    <t>P600_W_WSN_MN</t>
+  </si>
+  <si>
+    <t>P600_W_WSC_MN</t>
+  </si>
+  <si>
+    <t>P1000_W_WSC_MN</t>
+  </si>
+  <si>
+    <t>P1000_W_WSN_MN</t>
+  </si>
+  <si>
+    <t>N_WN_WSC_I(mm)</t>
+  </si>
+  <si>
+    <t>N_WN_WSC_I(%)</t>
   </si>
 </sst>
 </file>
@@ -1836,8 +1875,8 @@
   </sheetPr>
   <dimension ref="A1:DG77"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="CR1" zoomScale="84" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="DC3" sqref="DC3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1892,7 +1931,7 @@
         <v>94</v>
       </c>
       <c r="H1" s="35" t="s">
-        <v>246</v>
+        <v>231</v>
       </c>
       <c r="I1" s="35" t="s">
         <v>113</v>
@@ -1928,280 +1967,280 @@
         <v>166</v>
       </c>
       <c r="T1" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="U1" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="V1" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="W1" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="V1" s="5" t="s">
+      <c r="X1" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="W1" s="6" t="s">
+      <c r="Y1" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="Z1" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="Y1" s="5" t="s">
+      <c r="AA1" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="Z1" s="5" t="s">
+      <c r="AB1" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="AA1" s="5" t="s">
+      <c r="AC1" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="AB1" s="5" t="s">
+      <c r="AD1" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="AC1" s="5" t="s">
+      <c r="AE1" s="5" t="s">
         <v>176</v>
       </c>
-      <c r="AD1" s="5" t="s">
+      <c r="AF1" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="AE1" s="5" t="s">
+      <c r="AG1" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="AH1" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="AI1" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="AF1" s="5" t="s">
+      <c r="AJ1" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="AG1" s="5" t="s">
+      <c r="AK1" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="AH1" s="5" t="s">
+      <c r="AL1" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="AI1" s="5" t="s">
+      <c r="AM1" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="AJ1" s="5" t="s">
+      <c r="AN1" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="AK1" s="6" t="s">
+      <c r="AO1" s="5" t="s">
         <v>184</v>
       </c>
-      <c r="AL1" s="4" t="s">
+      <c r="AP1" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="AM1" s="5" t="s">
+      <c r="AQ1" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="AN1" s="5" t="s">
+      <c r="AR1" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="AO1" s="5" t="s">
+      <c r="AS1" s="5" t="s">
         <v>188</v>
       </c>
-      <c r="AP1" s="5" t="s">
+      <c r="AT1" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="AQ1" s="5" t="s">
+      <c r="AU1" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="AV1" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="AW1" s="5" t="s">
         <v>190</v>
       </c>
-      <c r="AR1" s="5" t="s">
+      <c r="AX1" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="AS1" s="5" t="s">
+      <c r="AY1" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="AZ1" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="BA1" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="BB1" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="BC1" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="BD1" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="BE1" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="BF1" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="BG1" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="BH1" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="BI1" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="BJ1" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="BK1" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="BL1" s="6" t="s">
+        <v>243</v>
+      </c>
+      <c r="BM1" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="AT1" s="5" t="s">
+      <c r="BN1" s="5" t="s">
         <v>193</v>
       </c>
-      <c r="AU1" s="5" t="s">
+      <c r="BO1" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="AV1" s="5" t="s">
+      <c r="BP1" s="5" t="s">
         <v>195</v>
       </c>
-      <c r="AW1" s="5" t="s">
+      <c r="BQ1" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="AX1" s="6" t="s">
+      <c r="BR1" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="AY1" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="AZ1" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="BA1" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="BB1" s="5" t="s">
-        <v>160</v>
-      </c>
-      <c r="BC1" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="BD1" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="BE1" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="BF1" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="BG1" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="BH1" s="5" t="s">
-        <v>167</v>
-      </c>
-      <c r="BI1" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="BJ1" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="BK1" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="BL1" s="6" t="s">
+      <c r="BS1" s="5" t="s">
         <v>198</v>
       </c>
-      <c r="BM1" s="4" t="s">
+      <c r="BT1" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="BN1" s="5" t="s">
+      <c r="BU1" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="BV1" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="BW1" s="5" t="s">
         <v>200</v>
       </c>
-      <c r="BO1" s="5" t="s">
+      <c r="BX1" s="6" t="s">
         <v>201</v>
       </c>
-      <c r="BP1" s="5" t="s">
+      <c r="BY1" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="BQ1" s="5" t="s">
+      <c r="BZ1" s="5" t="s">
         <v>203</v>
       </c>
-      <c r="BR1" s="5" t="s">
+      <c r="CA1" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="BS1" s="5" t="s">
+      <c r="CB1" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="BT1" s="5" t="s">
+      <c r="CC1" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="BU1" s="5" t="s">
-        <v>243</v>
-      </c>
-      <c r="BV1" s="5" t="s">
-        <v>244</v>
-      </c>
-      <c r="BW1" s="5" t="s">
+      <c r="CD1" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="BX1" s="6" t="s">
+      <c r="CE1" s="5" t="s">
         <v>208</v>
       </c>
-      <c r="BY1" s="4" t="s">
+      <c r="CF1" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="BZ1" s="5" t="s">
+      <c r="CG1" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="CH1" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="CI1" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="CA1" s="5" t="s">
+      <c r="CJ1" s="6" t="s">
         <v>211</v>
       </c>
-      <c r="CB1" s="5" t="s">
+      <c r="CK1" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="CC1" s="5" t="s">
+      <c r="CL1" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="CD1" s="5" t="s">
+      <c r="CM1" s="5" t="s">
         <v>214</v>
       </c>
-      <c r="CE1" s="5" t="s">
+      <c r="CN1" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="CF1" s="5" t="s">
+      <c r="CO1" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="CG1" s="5" t="s">
+      <c r="CP1" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="CH1" s="5" t="s">
+      <c r="CQ1" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="CI1" s="5" t="s">
+      <c r="CR1" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="CJ1" s="6" t="s">
+      <c r="CS1" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="CT1" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="CU1" s="5" t="s">
         <v>220</v>
       </c>
-      <c r="CK1" s="4" t="s">
+      <c r="CV1" s="6" t="s">
         <v>221</v>
       </c>
-      <c r="CL1" s="5" t="s">
+      <c r="CW1" s="5" t="s">
         <v>222</v>
       </c>
-      <c r="CM1" s="5" t="s">
+      <c r="CX1" s="5" t="s">
         <v>223</v>
       </c>
-      <c r="CN1" s="5" t="s">
+      <c r="CY1" s="5" t="s">
         <v>224</v>
       </c>
-      <c r="CO1" s="5" t="s">
+      <c r="CZ1" s="5" t="s">
         <v>225</v>
       </c>
-      <c r="CP1" s="5" t="s">
+      <c r="DA1" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="DB1" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="DC1" s="5" t="s">
         <v>226</v>
       </c>
-      <c r="CQ1" s="5" t="s">
+      <c r="DD1" s="5" t="s">
         <v>227</v>
       </c>
-      <c r="CR1" s="5" t="s">
+      <c r="DE1" s="5" t="s">
         <v>228</v>
       </c>
-      <c r="CS1" s="5" t="s">
+      <c r="DF1" s="5" t="s">
         <v>229</v>
       </c>
-      <c r="CT1" s="5" t="s">
-        <v>245</v>
-      </c>
-      <c r="CU1" s="5" t="s">
+      <c r="DG1" s="5" t="s">
         <v>230</v>
-      </c>
-      <c r="CV1" s="6" t="s">
-        <v>231</v>
-      </c>
-      <c r="CW1" s="5" t="s">
-        <v>232</v>
-      </c>
-      <c r="CX1" s="5" t="s">
-        <v>233</v>
-      </c>
-      <c r="CY1" s="5" t="s">
-        <v>234</v>
-      </c>
-      <c r="CZ1" s="5" t="s">
-        <v>235</v>
-      </c>
-      <c r="DA1" s="5" t="s">
-        <v>236</v>
-      </c>
-      <c r="DB1" s="5" t="s">
-        <v>242</v>
-      </c>
-      <c r="DC1" s="5" t="s">
-        <v>237</v>
-      </c>
-      <c r="DD1" s="5" t="s">
-        <v>238</v>
-      </c>
-      <c r="DE1" s="5" t="s">
-        <v>239</v>
-      </c>
-      <c r="DF1" s="5" t="s">
-        <v>240</v>
-      </c>
-      <c r="DG1" s="5" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="2" spans="1:111" ht="15" thickBot="1" x14ac:dyDescent="0.4">

</xml_diff>